<commit_message>
integrated results in one word file
</commit_message>
<xml_diff>
--- a/EJBComponents/ImageProcessingBenchmark/stats/analysis/benchmarkPolicyAnalysis/fullResourceAllocation.xlsx
+++ b/EJBComponents/ImageProcessingBenchmark/stats/analysis/benchmarkPolicyAnalysis/fullResourceAllocation.xlsx
@@ -398,23 +398,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,8 +407,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1282,11 +1282,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1674799568"/>
-        <c:axId val="-1674801200"/>
+        <c:axId val="1072163744"/>
+        <c:axId val="1072167008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1674799568"/>
+        <c:axId val="1072163744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1422,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674801200"/>
+        <c:crossAx val="1072167008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1430,7 +1430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674801200"/>
+        <c:axId val="1072167008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="550"/>
@@ -1563,7 +1563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674799568"/>
+        <c:crossAx val="1072163744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -2097,11 +2097,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674801744"/>
-        <c:axId val="-1674802832"/>
+        <c:axId val="771827248"/>
+        <c:axId val="771828336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674801744"/>
+        <c:axId val="771827248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674802832"/>
+        <c:crossAx val="771828336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2215,7 +2215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674802832"/>
+        <c:axId val="771828336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -2347,7 +2347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674801744"/>
+        <c:crossAx val="771827248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -2839,11 +2839,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674802288"/>
-        <c:axId val="-1674800112"/>
+        <c:axId val="771833232"/>
+        <c:axId val="771830512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674802288"/>
+        <c:axId val="771833232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2949,7 +2949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674800112"/>
+        <c:crossAx val="771830512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2957,7 +2957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674800112"/>
+        <c:axId val="771830512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -3089,7 +3089,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674802288"/>
+        <c:crossAx val="771833232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -3581,11 +3581,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1671507024"/>
-        <c:axId val="-1671505936"/>
+        <c:axId val="771833776"/>
+        <c:axId val="771818544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1671507024"/>
+        <c:axId val="771833776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3691,7 +3691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671505936"/>
+        <c:crossAx val="771818544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3699,7 +3699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1671505936"/>
+        <c:axId val="771818544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -3831,7 +3831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671507024"/>
+        <c:crossAx val="771833776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -4316,11 +4316,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1671515184"/>
-        <c:axId val="-1671512464"/>
+        <c:axId val="1049741120"/>
+        <c:axId val="1049734592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1671515184"/>
+        <c:axId val="1049741120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4423,7 +4423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671512464"/>
+        <c:crossAx val="1049734592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4431,7 +4431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1671512464"/>
+        <c:axId val="1049734592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -4562,7 +4562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671515184"/>
+        <c:crossAx val="1049741120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -5047,11 +5047,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1671505392"/>
-        <c:axId val="-1671509744"/>
+        <c:axId val="1049728608"/>
+        <c:axId val="1049729152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1671505392"/>
+        <c:axId val="1049728608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5154,7 +5154,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671509744"/>
+        <c:crossAx val="1049729152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5162,7 +5162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1671509744"/>
+        <c:axId val="1049729152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -5293,7 +5293,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671505392"/>
+        <c:crossAx val="1049728608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -6147,11 +6147,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1674800656"/>
-        <c:axId val="-1674792496"/>
+        <c:axId val="1072164288"/>
+        <c:axId val="1072165376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1674800656"/>
+        <c:axId val="1072164288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6287,7 +6287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674792496"/>
+        <c:crossAx val="1072165376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6295,7 +6295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674792496"/>
+        <c:axId val="1072165376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1100"/>
@@ -6428,7 +6428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674800656"/>
+        <c:crossAx val="1072164288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -6962,11 +6962,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674794672"/>
-        <c:axId val="-1674793584"/>
+        <c:axId val="1072156672"/>
+        <c:axId val="1072167552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674794672"/>
+        <c:axId val="1072156672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7072,7 +7072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674793584"/>
+        <c:crossAx val="1072167552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7080,7 +7080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674793584"/>
+        <c:axId val="1072167552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -7211,9 +7211,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674794672"/>
+        <c:crossAx val="1072156672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -7702,11 +7703,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674791952"/>
-        <c:axId val="-1674799024"/>
+        <c:axId val="1072168096"/>
+        <c:axId val="1072157760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674791952"/>
+        <c:axId val="1072168096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7812,7 +7813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674799024"/>
+        <c:crossAx val="1072157760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7820,7 +7821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674799024"/>
+        <c:axId val="1072157760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -7951,9 +7952,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674791952"/>
+        <c:crossAx val="1072168096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -8442,11 +8444,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674798480"/>
-        <c:axId val="-1674795760"/>
+        <c:axId val="1072168640"/>
+        <c:axId val="1072169184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674798480"/>
+        <c:axId val="1072168640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8552,7 +8554,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674795760"/>
+        <c:crossAx val="1072169184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8560,7 +8562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674795760"/>
+        <c:axId val="1072169184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -8691,9 +8693,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674798480"/>
+        <c:crossAx val="1072168640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9182,11 +9185,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674791408"/>
-        <c:axId val="-1674805552"/>
+        <c:axId val="1072169728"/>
+        <c:axId val="1072170272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674791408"/>
+        <c:axId val="1072169728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9292,7 +9295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674805552"/>
+        <c:crossAx val="1072170272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9300,7 +9303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674805552"/>
+        <c:axId val="1072170272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -9431,9 +9434,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674791408"/>
+        <c:crossAx val="1072169728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9922,11 +9926,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674790864"/>
-        <c:axId val="-1674795216"/>
+        <c:axId val="1072170816"/>
+        <c:axId val="1072156128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674790864"/>
+        <c:axId val="1072170816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10032,7 +10036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674795216"/>
+        <c:crossAx val="1072156128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10040,7 +10044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674795216"/>
+        <c:axId val="1072156128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -10171,9 +10175,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674790864"/>
+        <c:crossAx val="1072170816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -10662,11 +10667,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674805008"/>
-        <c:axId val="-1674804464"/>
+        <c:axId val="771822896"/>
+        <c:axId val="771827792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674805008"/>
+        <c:axId val="771822896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10772,7 +10777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674804464"/>
+        <c:crossAx val="771827792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10780,7 +10785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674804464"/>
+        <c:axId val="771827792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -10912,7 +10917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674805008"/>
+        <c:crossAx val="771822896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -11404,11 +11409,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1674803920"/>
-        <c:axId val="-1674803376"/>
+        <c:axId val="771826704"/>
+        <c:axId val="771832688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1674803920"/>
+        <c:axId val="771826704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11514,7 +11519,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674803376"/>
+        <c:crossAx val="771832688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11522,7 +11527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1674803376"/>
+        <c:axId val="771832688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -11653,7 +11658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1674803920"/>
+        <c:crossAx val="771826704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -20065,8 +20070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BV67" sqref="BV67"/>
+    <sheetView tabSelected="1" topLeftCell="BV142" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="EC34" sqref="EC34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20084,35 +20089,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
       <c r="AD1" s="26" t="s">
         <v>44</v>
       </c>
@@ -20120,42 +20125,42 @@
       <c r="AF1" s="26"/>
       <c r="AG1" s="26"/>
       <c r="AH1" s="26"/>
-      <c r="AJ1" s="22" t="s">
+      <c r="AJ1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="22"/>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22"/>
-      <c r="BN1" s="22"/>
-      <c r="BO1" s="22"/>
-      <c r="BP1" s="22"/>
-      <c r="BQ1" s="22"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
     </row>
     <row r="2" spans="1:69" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -20251,49 +20256,49 @@
       <c r="AJ2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AK2" s="25" t="s">
+      <c r="AK2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
       <c r="AP2" s="8"/>
       <c r="AQ2" s="8"/>
-      <c r="AR2" s="25" t="s">
+      <c r="AR2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="25"/>
-      <c r="AV2" s="25"/>
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
       <c r="AW2" s="8"/>
       <c r="AX2" s="8"/>
-      <c r="AY2" s="25" t="s">
+      <c r="AY2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
       <c r="BD2" s="8"/>
       <c r="BE2" s="8"/>
-      <c r="BF2" s="25" t="s">
+      <c r="BF2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="BG2" s="25"/>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="25"/>
+      <c r="BG2" s="27"/>
+      <c r="BH2" s="27"/>
+      <c r="BI2" s="27"/>
+      <c r="BJ2" s="27"/>
       <c r="BK2" s="8"/>
       <c r="BL2" s="8"/>
-      <c r="BM2" s="25" t="s">
+      <c r="BM2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="BN2" s="25"/>
-      <c r="BO2" s="25"/>
-      <c r="BP2" s="25"/>
-      <c r="BQ2" s="25"/>
+      <c r="BN2" s="27"/>
+      <c r="BO2" s="27"/>
+      <c r="BP2" s="27"/>
+      <c r="BQ2" s="27"/>
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -20582,35 +20587,35 @@
       </c>
     </row>
     <row r="5" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
-      <c r="AA5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
       <c r="AJ5" s="11">
         <v>2</v>
       </c>
@@ -21367,35 +21372,35 @@
       </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
       <c r="AJ10" s="13">
         <v>12</v>
       </c>
@@ -22001,70 +22006,70 @@
       </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
-      <c r="AA15" s="28"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
       <c r="AJ15" s="8"/>
-      <c r="AK15" s="27" t="s">
+      <c r="AK15" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="AL15" s="27"/>
-      <c r="AM15" s="27"/>
-      <c r="AN15" s="27"/>
-      <c r="AO15" s="27"/>
+      <c r="AL15" s="28"/>
+      <c r="AM15" s="28"/>
+      <c r="AN15" s="28"/>
+      <c r="AO15" s="28"/>
       <c r="AP15" s="8"/>
       <c r="AQ15" s="8"/>
-      <c r="AR15" s="27" t="s">
+      <c r="AR15" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="AS15" s="27"/>
-      <c r="AT15" s="27"/>
-      <c r="AU15" s="27"/>
-      <c r="AV15" s="27"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="28"/>
+      <c r="AV15" s="28"/>
       <c r="AW15" s="8"/>
       <c r="AX15" s="8"/>
-      <c r="AY15" s="22" t="s">
+      <c r="AY15" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="AZ15" s="22"/>
-      <c r="BA15" s="22"/>
-      <c r="BB15" s="22"/>
-      <c r="BC15" s="22"/>
+      <c r="AZ15" s="25"/>
+      <c r="BA15" s="25"/>
+      <c r="BB15" s="25"/>
+      <c r="BC15" s="25"/>
       <c r="BD15" s="8"/>
       <c r="BE15" s="8"/>
-      <c r="BF15" s="27" t="s">
+      <c r="BF15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="BG15" s="27"/>
-      <c r="BH15" s="27"/>
-      <c r="BI15" s="27"/>
-      <c r="BJ15" s="27"/>
+      <c r="BG15" s="28"/>
+      <c r="BH15" s="28"/>
+      <c r="BI15" s="28"/>
+      <c r="BJ15" s="28"/>
     </row>
     <row r="16" spans="1:69" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -22161,32 +22166,32 @@
         <v>48</v>
       </c>
       <c r="AJ16" s="12"/>
-      <c r="AK16" s="27"/>
-      <c r="AL16" s="27"/>
-      <c r="AM16" s="27"/>
-      <c r="AN16" s="27"/>
-      <c r="AO16" s="27"/>
+      <c r="AK16" s="28"/>
+      <c r="AL16" s="28"/>
+      <c r="AM16" s="28"/>
+      <c r="AN16" s="28"/>
+      <c r="AO16" s="28"/>
       <c r="AP16" s="12"/>
       <c r="AQ16" s="12"/>
-      <c r="AR16" s="27"/>
-      <c r="AS16" s="27"/>
-      <c r="AT16" s="27"/>
-      <c r="AU16" s="27"/>
-      <c r="AV16" s="27"/>
+      <c r="AR16" s="28"/>
+      <c r="AS16" s="28"/>
+      <c r="AT16" s="28"/>
+      <c r="AU16" s="28"/>
+      <c r="AV16" s="28"/>
       <c r="AW16" s="12"/>
       <c r="AX16" s="12"/>
-      <c r="AY16" s="22"/>
-      <c r="AZ16" s="22"/>
-      <c r="BA16" s="22"/>
-      <c r="BB16" s="22"/>
-      <c r="BC16" s="22"/>
+      <c r="AY16" s="25"/>
+      <c r="AZ16" s="25"/>
+      <c r="BA16" s="25"/>
+      <c r="BB16" s="25"/>
+      <c r="BC16" s="25"/>
       <c r="BD16" s="12"/>
       <c r="BE16" s="12"/>
-      <c r="BF16" s="27"/>
-      <c r="BG16" s="27"/>
-      <c r="BH16" s="27"/>
-      <c r="BI16" s="27"/>
-      <c r="BJ16" s="27"/>
+      <c r="BF16" s="28"/>
+      <c r="BG16" s="28"/>
+      <c r="BH16" s="28"/>
+      <c r="BI16" s="28"/>
+      <c r="BJ16" s="28"/>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -22636,24 +22641,24 @@
       </c>
     </row>
     <row r="20" spans="1:62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
       <c r="AJ20" s="11">
         <v>6</v>
       </c>
@@ -22745,35 +22750,35 @@
       </c>
     </row>
     <row r="21" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="30"/>
-      <c r="Z21" s="30"/>
-      <c r="AA21" s="30"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="22"/>
+      <c r="V21" s="22"/>
+      <c r="W21" s="22"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="22"/>
       <c r="AJ21" s="13">
         <v>8</v>
       </c>
@@ -23672,35 +23677,35 @@
       </c>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="28"/>
-      <c r="V28" s="28"/>
-      <c r="W28" s="28"/>
-      <c r="X28" s="28"/>
-      <c r="Y28" s="28"/>
-      <c r="Z28" s="28"/>
-      <c r="AA28" s="28"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -23885,23 +23890,23 @@
       <c r="AP30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AQ30" s="22" t="s">
+      <c r="AQ30" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AR30" s="22"/>
-      <c r="AS30" s="22"/>
-      <c r="AT30" s="22"/>
-      <c r="AU30" s="22"/>
+      <c r="AR30" s="25"/>
+      <c r="AS30" s="25"/>
+      <c r="AT30" s="25"/>
+      <c r="AU30" s="25"/>
       <c r="BC30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="BD30" s="22" t="s">
+      <c r="BD30" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="BE30" s="22"/>
-      <c r="BF30" s="22"/>
-      <c r="BG30" s="22"/>
-      <c r="BH30" s="22"/>
+      <c r="BE30" s="25"/>
+      <c r="BF30" s="25"/>
+      <c r="BG30" s="25"/>
+      <c r="BH30" s="25"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
@@ -24346,24 +24351,24 @@
       </c>
     </row>
     <row r="35" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
       <c r="AP35" s="11">
         <v>6</v>
       </c>
@@ -24412,35 +24417,35 @@
       </c>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="30"/>
-      <c r="Z36" s="30"/>
-      <c r="AA36" s="30"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+      <c r="AA36" s="22"/>
       <c r="AP36" s="13">
         <v>8</v>
       </c>
@@ -25304,35 +25309,35 @@
       </c>
     </row>
     <row r="45" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="28"/>
-      <c r="Q45" s="28"/>
-      <c r="R45" s="28"/>
-      <c r="S45" s="28"/>
-      <c r="T45" s="28"/>
-      <c r="U45" s="28"/>
-      <c r="V45" s="28"/>
-      <c r="W45" s="28"/>
-      <c r="X45" s="28"/>
-      <c r="Y45" s="28"/>
-      <c r="Z45" s="28"/>
-      <c r="AA45" s="28"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="23"/>
+      <c r="S45" s="23"/>
+      <c r="T45" s="23"/>
+      <c r="U45" s="23"/>
+      <c r="V45" s="23"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
+      <c r="Z45" s="23"/>
+      <c r="AA45" s="23"/>
     </row>
     <row r="46" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
@@ -25694,42 +25699,42 @@
         <f t="shared" si="84"/>
         <v>2.4</v>
       </c>
-      <c r="AJ49" s="24" t="s">
+      <c r="AJ49" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="AK49" s="24"/>
-      <c r="AL49" s="24"/>
-      <c r="AM49" s="24"/>
-      <c r="AN49" s="24"/>
-      <c r="AO49" s="24"/>
-      <c r="AP49" s="24"/>
-      <c r="AQ49" s="24"/>
-      <c r="AR49" s="24"/>
-      <c r="AS49" s="24"/>
-      <c r="AT49" s="24"/>
-      <c r="AU49" s="24"/>
-      <c r="AV49" s="24"/>
-      <c r="AW49" s="24"/>
-      <c r="AX49" s="24"/>
-      <c r="AY49" s="24"/>
-      <c r="AZ49" s="24"/>
-      <c r="BA49" s="24"/>
-      <c r="BB49" s="24"/>
-      <c r="BC49" s="24"/>
-      <c r="BD49" s="24"/>
-      <c r="BE49" s="24"/>
-      <c r="BF49" s="24"/>
-      <c r="BG49" s="24"/>
-      <c r="BH49" s="24"/>
-      <c r="BI49" s="24"/>
-      <c r="BJ49" s="24"/>
-      <c r="BK49" s="24"/>
-      <c r="BL49" s="24"/>
-      <c r="BM49" s="24"/>
-      <c r="BN49" s="24"/>
-      <c r="BO49" s="24"/>
-      <c r="BP49" s="24"/>
-      <c r="BQ49" s="24"/>
+      <c r="AK49" s="30"/>
+      <c r="AL49" s="30"/>
+      <c r="AM49" s="30"/>
+      <c r="AN49" s="30"/>
+      <c r="AO49" s="30"/>
+      <c r="AP49" s="30"/>
+      <c r="AQ49" s="30"/>
+      <c r="AR49" s="30"/>
+      <c r="AS49" s="30"/>
+      <c r="AT49" s="30"/>
+      <c r="AU49" s="30"/>
+      <c r="AV49" s="30"/>
+      <c r="AW49" s="30"/>
+      <c r="AX49" s="30"/>
+      <c r="AY49" s="30"/>
+      <c r="AZ49" s="30"/>
+      <c r="BA49" s="30"/>
+      <c r="BB49" s="30"/>
+      <c r="BC49" s="30"/>
+      <c r="BD49" s="30"/>
+      <c r="BE49" s="30"/>
+      <c r="BF49" s="30"/>
+      <c r="BG49" s="30"/>
+      <c r="BH49" s="30"/>
+      <c r="BI49" s="30"/>
+      <c r="BJ49" s="30"/>
+      <c r="BK49" s="30"/>
+      <c r="BL49" s="30"/>
+      <c r="BM49" s="30"/>
+      <c r="BN49" s="30"/>
+      <c r="BO49" s="30"/>
+      <c r="BP49" s="30"/>
+      <c r="BQ49" s="30"/>
     </row>
     <row r="50" spans="1:69" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
@@ -25823,49 +25828,49 @@
       <c r="AJ50" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AK50" s="25" t="s">
+      <c r="AK50" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AL50" s="25"/>
-      <c r="AM50" s="25"/>
-      <c r="AN50" s="25"/>
-      <c r="AO50" s="25"/>
+      <c r="AL50" s="27"/>
+      <c r="AM50" s="27"/>
+      <c r="AN50" s="27"/>
+      <c r="AO50" s="27"/>
       <c r="AP50" s="8"/>
       <c r="AQ50" s="8"/>
-      <c r="AR50" s="25" t="s">
+      <c r="AR50" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AS50" s="25"/>
-      <c r="AT50" s="25"/>
-      <c r="AU50" s="25"/>
-      <c r="AV50" s="25"/>
+      <c r="AS50" s="27"/>
+      <c r="AT50" s="27"/>
+      <c r="AU50" s="27"/>
+      <c r="AV50" s="27"/>
       <c r="AW50" s="8"/>
       <c r="AX50" s="8"/>
-      <c r="AY50" s="25" t="s">
+      <c r="AY50" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AZ50" s="25"/>
-      <c r="BA50" s="25"/>
-      <c r="BB50" s="25"/>
-      <c r="BC50" s="25"/>
+      <c r="AZ50" s="27"/>
+      <c r="BA50" s="27"/>
+      <c r="BB50" s="27"/>
+      <c r="BC50" s="27"/>
       <c r="BD50" s="8"/>
       <c r="BE50" s="8"/>
-      <c r="BF50" s="25" t="s">
+      <c r="BF50" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="BG50" s="25"/>
-      <c r="BH50" s="25"/>
-      <c r="BI50" s="25"/>
-      <c r="BJ50" s="25"/>
+      <c r="BG50" s="27"/>
+      <c r="BH50" s="27"/>
+      <c r="BI50" s="27"/>
+      <c r="BJ50" s="27"/>
       <c r="BK50" s="8"/>
       <c r="BL50" s="8"/>
-      <c r="BM50" s="25" t="s">
+      <c r="BM50" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="BN50" s="25"/>
-      <c r="BO50" s="25"/>
-      <c r="BP50" s="25"/>
-      <c r="BQ50" s="25"/>
+      <c r="BN50" s="27"/>
+      <c r="BO50" s="27"/>
+      <c r="BP50" s="27"/>
+      <c r="BQ50" s="27"/>
     </row>
     <row r="51" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
@@ -26356,24 +26361,24 @@
       </c>
     </row>
     <row r="54" spans="1:69" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
-      <c r="O54" s="29"/>
-      <c r="P54" s="29"/>
-      <c r="Q54" s="29"/>
-      <c r="R54" s="29"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="24"/>
       <c r="AJ54" s="13">
         <v>4</v>
       </c>
@@ -26487,35 +26492,35 @@
       </c>
     </row>
     <row r="55" spans="1:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="30"/>
-      <c r="O55" s="30"/>
-      <c r="P55" s="30"/>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="30"/>
-      <c r="S55" s="30"/>
-      <c r="T55" s="30"/>
-      <c r="U55" s="30"/>
-      <c r="V55" s="30"/>
-      <c r="W55" s="30"/>
-      <c r="X55" s="30"/>
-      <c r="Y55" s="30"/>
-      <c r="Z55" s="30"/>
-      <c r="AA55" s="30"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+      <c r="Q55" s="22"/>
+      <c r="R55" s="22"/>
+      <c r="S55" s="22"/>
+      <c r="T55" s="22"/>
+      <c r="U55" s="22"/>
+      <c r="V55" s="22"/>
+      <c r="W55" s="22"/>
+      <c r="X55" s="22"/>
+      <c r="Y55" s="22"/>
+      <c r="Z55" s="22"/>
+      <c r="AA55" s="22"/>
       <c r="AJ55" s="11">
         <v>6</v>
       </c>
@@ -27904,40 +27909,40 @@
         <v>90.6</v>
       </c>
       <c r="AJ63" s="8"/>
-      <c r="AK63" s="23" t="s">
+      <c r="AK63" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="AL63" s="23"/>
-      <c r="AM63" s="23"/>
-      <c r="AN63" s="23"/>
-      <c r="AO63" s="23"/>
+      <c r="AL63" s="29"/>
+      <c r="AM63" s="29"/>
+      <c r="AN63" s="29"/>
+      <c r="AO63" s="29"/>
       <c r="AP63" s="8"/>
       <c r="AQ63" s="8"/>
-      <c r="AR63" s="23" t="s">
+      <c r="AR63" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AS63" s="23"/>
-      <c r="AT63" s="23"/>
-      <c r="AU63" s="23"/>
-      <c r="AV63" s="23"/>
+      <c r="AS63" s="29"/>
+      <c r="AT63" s="29"/>
+      <c r="AU63" s="29"/>
+      <c r="AV63" s="29"/>
       <c r="AW63" s="8"/>
       <c r="AX63" s="8"/>
-      <c r="AY63" s="24" t="s">
+      <c r="AY63" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="AZ63" s="24"/>
-      <c r="BA63" s="24"/>
-      <c r="BB63" s="24"/>
-      <c r="BC63" s="24"/>
+      <c r="AZ63" s="30"/>
+      <c r="BA63" s="30"/>
+      <c r="BB63" s="30"/>
+      <c r="BC63" s="30"/>
       <c r="BD63" s="8"/>
       <c r="BE63" s="8"/>
-      <c r="BF63" s="23" t="s">
+      <c r="BF63" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="BG63" s="23"/>
-      <c r="BH63" s="23"/>
-      <c r="BI63" s="23"/>
-      <c r="BJ63" s="23"/>
+      <c r="BG63" s="29"/>
+      <c r="BH63" s="29"/>
+      <c r="BI63" s="29"/>
+      <c r="BJ63" s="29"/>
     </row>
     <row r="64" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
@@ -28029,32 +28034,32 @@
         <v>91</v>
       </c>
       <c r="AJ64" s="12"/>
-      <c r="AK64" s="23"/>
-      <c r="AL64" s="23"/>
-      <c r="AM64" s="23"/>
-      <c r="AN64" s="23"/>
-      <c r="AO64" s="23"/>
+      <c r="AK64" s="29"/>
+      <c r="AL64" s="29"/>
+      <c r="AM64" s="29"/>
+      <c r="AN64" s="29"/>
+      <c r="AO64" s="29"/>
       <c r="AP64" s="12"/>
       <c r="AQ64" s="12"/>
-      <c r="AR64" s="23"/>
-      <c r="AS64" s="23"/>
-      <c r="AT64" s="23"/>
-      <c r="AU64" s="23"/>
-      <c r="AV64" s="23"/>
+      <c r="AR64" s="29"/>
+      <c r="AS64" s="29"/>
+      <c r="AT64" s="29"/>
+      <c r="AU64" s="29"/>
+      <c r="AV64" s="29"/>
       <c r="AW64" s="12"/>
       <c r="AX64" s="12"/>
-      <c r="AY64" s="24"/>
-      <c r="AZ64" s="24"/>
-      <c r="BA64" s="24"/>
-      <c r="BB64" s="24"/>
-      <c r="BC64" s="24"/>
+      <c r="AY64" s="30"/>
+      <c r="AZ64" s="30"/>
+      <c r="BA64" s="30"/>
+      <c r="BB64" s="30"/>
+      <c r="BC64" s="30"/>
       <c r="BD64" s="12"/>
       <c r="BE64" s="12"/>
-      <c r="BF64" s="23"/>
-      <c r="BG64" s="23"/>
-      <c r="BH64" s="23"/>
-      <c r="BI64" s="23"/>
-      <c r="BJ64" s="23"/>
+      <c r="BF64" s="29"/>
+      <c r="BG64" s="29"/>
+      <c r="BH64" s="29"/>
+      <c r="BI64" s="29"/>
+      <c r="BJ64" s="29"/>
       <c r="BK64" s="1"/>
       <c r="BL64" s="1"/>
       <c r="BM64" s="1"/>
@@ -28155,35 +28160,35 @@
       </c>
     </row>
     <row r="66" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="28"/>
-      <c r="K66" s="28"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="28"/>
-      <c r="N66" s="28"/>
-      <c r="O66" s="28"/>
-      <c r="P66" s="28"/>
-      <c r="Q66" s="28"/>
-      <c r="R66" s="28"/>
-      <c r="S66" s="28"/>
-      <c r="T66" s="28"/>
-      <c r="U66" s="28"/>
-      <c r="V66" s="28"/>
-      <c r="W66" s="28"/>
-      <c r="X66" s="28"/>
-      <c r="Y66" s="28"/>
-      <c r="Z66" s="28"/>
-      <c r="AA66" s="28"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="23"/>
+      <c r="N66" s="23"/>
+      <c r="O66" s="23"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="23"/>
+      <c r="S66" s="23"/>
+      <c r="T66" s="23"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="23"/>
+      <c r="W66" s="23"/>
+      <c r="X66" s="23"/>
+      <c r="Y66" s="23"/>
+      <c r="Z66" s="23"/>
+      <c r="AA66" s="23"/>
       <c r="AJ66" s="11">
         <v>2</v>
       </c>
@@ -29709,75 +29714,75 @@
       </c>
     </row>
     <row r="77" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
-      <c r="I77" s="29"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="29"/>
-      <c r="L77" s="29"/>
-      <c r="M77" s="29"/>
-      <c r="N77" s="29"/>
-      <c r="O77" s="29"/>
-      <c r="P77" s="29"/>
-      <c r="Q77" s="29"/>
-      <c r="R77" s="29"/>
+      <c r="A77" s="24"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="24"/>
+      <c r="L77" s="24"/>
+      <c r="M77" s="24"/>
+      <c r="N77" s="24"/>
+      <c r="O77" s="24"/>
+      <c r="P77" s="24"/>
+      <c r="Q77" s="24"/>
+      <c r="R77" s="24"/>
     </row>
     <row r="78" spans="1:62" ht="60" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="30"/>
-      <c r="G78" s="30"/>
-      <c r="H78" s="30"/>
-      <c r="I78" s="30"/>
-      <c r="J78" s="30"/>
-      <c r="K78" s="30"/>
-      <c r="L78" s="30"/>
-      <c r="M78" s="30"/>
-      <c r="N78" s="30"/>
-      <c r="O78" s="30"/>
-      <c r="P78" s="30"/>
-      <c r="Q78" s="30"/>
-      <c r="R78" s="30"/>
-      <c r="S78" s="30"/>
-      <c r="T78" s="30"/>
-      <c r="U78" s="30"/>
-      <c r="V78" s="30"/>
-      <c r="W78" s="30"/>
-      <c r="X78" s="30"/>
-      <c r="Y78" s="30"/>
-      <c r="Z78" s="30"/>
-      <c r="AA78" s="30"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="22"/>
+      <c r="I78" s="22"/>
+      <c r="J78" s="22"/>
+      <c r="K78" s="22"/>
+      <c r="L78" s="22"/>
+      <c r="M78" s="22"/>
+      <c r="N78" s="22"/>
+      <c r="O78" s="22"/>
+      <c r="P78" s="22"/>
+      <c r="Q78" s="22"/>
+      <c r="R78" s="22"/>
+      <c r="S78" s="22"/>
+      <c r="T78" s="22"/>
+      <c r="U78" s="22"/>
+      <c r="V78" s="22"/>
+      <c r="W78" s="22"/>
+      <c r="X78" s="22"/>
+      <c r="Y78" s="22"/>
+      <c r="Z78" s="22"/>
+      <c r="AA78" s="22"/>
       <c r="AP78" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AQ78" s="24" t="s">
+      <c r="AQ78" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AR78" s="24"/>
-      <c r="AS78" s="24"/>
-      <c r="AT78" s="24"/>
-      <c r="AU78" s="24"/>
+      <c r="AR78" s="30"/>
+      <c r="AS78" s="30"/>
+      <c r="AT78" s="30"/>
+      <c r="AU78" s="30"/>
       <c r="BC78" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="BD78" s="24" t="s">
+      <c r="BD78" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="BE78" s="24"/>
-      <c r="BF78" s="24"/>
-      <c r="BG78" s="24"/>
-      <c r="BH78" s="24"/>
+      <c r="BE78" s="30"/>
+      <c r="BF78" s="30"/>
+      <c r="BG78" s="30"/>
+      <c r="BH78" s="30"/>
     </row>
     <row r="79" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
@@ -31217,35 +31222,35 @@
       </c>
     </row>
     <row r="91" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A91" s="28" t="s">
+      <c r="A91" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="28"/>
-      <c r="H91" s="28"/>
-      <c r="I91" s="28"/>
-      <c r="J91" s="28"/>
-      <c r="K91" s="28"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="28"/>
-      <c r="N91" s="28"/>
-      <c r="O91" s="28"/>
-      <c r="P91" s="28"/>
-      <c r="Q91" s="28"/>
-      <c r="R91" s="28"/>
-      <c r="S91" s="28"/>
-      <c r="T91" s="28"/>
-      <c r="U91" s="28"/>
-      <c r="V91" s="28"/>
-      <c r="W91" s="28"/>
-      <c r="X91" s="28"/>
-      <c r="Y91" s="28"/>
-      <c r="Z91" s="28"/>
-      <c r="AA91" s="28"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
+      <c r="J91" s="23"/>
+      <c r="K91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="23"/>
+      <c r="N91" s="23"/>
+      <c r="O91" s="23"/>
+      <c r="P91" s="23"/>
+      <c r="Q91" s="23"/>
+      <c r="R91" s="23"/>
+      <c r="S91" s="23"/>
+      <c r="T91" s="23"/>
+      <c r="U91" s="23"/>
+      <c r="V91" s="23"/>
+      <c r="W91" s="23"/>
+      <c r="X91" s="23"/>
+      <c r="Y91" s="23"/>
+      <c r="Z91" s="23"/>
+      <c r="AA91" s="23"/>
     </row>
     <row r="92" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
@@ -32668,55 +32673,55 @@
       </c>
     </row>
     <row r="104" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="29"/>
-      <c r="B104" s="29"/>
-      <c r="C104" s="29"/>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-      <c r="H104" s="29"/>
-      <c r="I104" s="29"/>
-      <c r="J104" s="29"/>
-      <c r="K104" s="29"/>
-      <c r="L104" s="29"/>
-      <c r="M104" s="29"/>
-      <c r="N104" s="29"/>
-      <c r="O104" s="29"/>
-      <c r="P104" s="29"/>
-      <c r="Q104" s="29"/>
-      <c r="R104" s="29"/>
+      <c r="A104" s="24"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="24"/>
+      <c r="K104" s="24"/>
+      <c r="L104" s="24"/>
+      <c r="M104" s="24"/>
+      <c r="N104" s="24"/>
+      <c r="O104" s="24"/>
+      <c r="P104" s="24"/>
+      <c r="Q104" s="24"/>
+      <c r="R104" s="24"/>
     </row>
     <row r="105" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+      <c r="A105" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B105" s="30"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="30"/>
-      <c r="E105" s="30"/>
-      <c r="F105" s="30"/>
-      <c r="G105" s="30"/>
-      <c r="H105" s="30"/>
-      <c r="I105" s="30"/>
-      <c r="J105" s="30"/>
-      <c r="K105" s="30"/>
-      <c r="L105" s="30"/>
-      <c r="M105" s="30"/>
-      <c r="N105" s="30"/>
-      <c r="O105" s="30"/>
-      <c r="P105" s="30"/>
-      <c r="Q105" s="30"/>
-      <c r="R105" s="30"/>
-      <c r="S105" s="30"/>
-      <c r="T105" s="30"/>
-      <c r="U105" s="30"/>
-      <c r="V105" s="30"/>
-      <c r="W105" s="30"/>
-      <c r="X105" s="30"/>
-      <c r="Y105" s="30"/>
-      <c r="Z105" s="30"/>
-      <c r="AA105" s="30"/>
+      <c r="B105" s="22"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
+      <c r="H105" s="22"/>
+      <c r="I105" s="22"/>
+      <c r="J105" s="22"/>
+      <c r="K105" s="22"/>
+      <c r="L105" s="22"/>
+      <c r="M105" s="22"/>
+      <c r="N105" s="22"/>
+      <c r="O105" s="22"/>
+      <c r="P105" s="22"/>
+      <c r="Q105" s="22"/>
+      <c r="R105" s="22"/>
+      <c r="S105" s="22"/>
+      <c r="T105" s="22"/>
+      <c r="U105" s="22"/>
+      <c r="V105" s="22"/>
+      <c r="W105" s="22"/>
+      <c r="X105" s="22"/>
+      <c r="Y105" s="22"/>
+      <c r="Z105" s="22"/>
+      <c r="AA105" s="22"/>
     </row>
     <row r="106" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
@@ -34317,35 +34322,35 @@
       </c>
     </row>
     <row r="120" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B120" s="28"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="28"/>
-      <c r="E120" s="28"/>
-      <c r="F120" s="28"/>
-      <c r="G120" s="28"/>
-      <c r="H120" s="28"/>
-      <c r="I120" s="28"/>
-      <c r="J120" s="28"/>
-      <c r="K120" s="28"/>
-      <c r="L120" s="28"/>
-      <c r="M120" s="28"/>
-      <c r="N120" s="28"/>
-      <c r="O120" s="28"/>
-      <c r="P120" s="28"/>
-      <c r="Q120" s="28"/>
-      <c r="R120" s="28"/>
-      <c r="S120" s="28"/>
-      <c r="T120" s="28"/>
-      <c r="U120" s="28"/>
-      <c r="V120" s="28"/>
-      <c r="W120" s="28"/>
-      <c r="X120" s="28"/>
-      <c r="Y120" s="28"/>
-      <c r="Z120" s="28"/>
-      <c r="AA120" s="28"/>
+      <c r="B120" s="23"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="23"/>
+      <c r="F120" s="23"/>
+      <c r="G120" s="23"/>
+      <c r="H120" s="23"/>
+      <c r="I120" s="23"/>
+      <c r="J120" s="23"/>
+      <c r="K120" s="23"/>
+      <c r="L120" s="23"/>
+      <c r="M120" s="23"/>
+      <c r="N120" s="23"/>
+      <c r="O120" s="23"/>
+      <c r="P120" s="23"/>
+      <c r="Q120" s="23"/>
+      <c r="R120" s="23"/>
+      <c r="S120" s="23"/>
+      <c r="T120" s="23"/>
+      <c r="U120" s="23"/>
+      <c r="V120" s="23"/>
+      <c r="W120" s="23"/>
+      <c r="X120" s="23"/>
+      <c r="Y120" s="23"/>
+      <c r="Z120" s="23"/>
+      <c r="AA120" s="23"/>
     </row>
     <row r="121" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
@@ -35519,55 +35524,55 @@
       </c>
     </row>
     <row r="135" spans="1:35" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="29"/>
-      <c r="B135" s="29"/>
-      <c r="C135" s="29"/>
-      <c r="D135" s="29"/>
-      <c r="E135" s="29"/>
-      <c r="F135" s="29"/>
-      <c r="G135" s="29"/>
-      <c r="H135" s="29"/>
-      <c r="I135" s="29"/>
-      <c r="J135" s="29"/>
-      <c r="K135" s="29"/>
-      <c r="L135" s="29"/>
-      <c r="M135" s="29"/>
-      <c r="N135" s="29"/>
-      <c r="O135" s="29"/>
-      <c r="P135" s="29"/>
-      <c r="Q135" s="29"/>
-      <c r="R135" s="29"/>
+      <c r="A135" s="24"/>
+      <c r="B135" s="24"/>
+      <c r="C135" s="24"/>
+      <c r="D135" s="24"/>
+      <c r="E135" s="24"/>
+      <c r="F135" s="24"/>
+      <c r="G135" s="24"/>
+      <c r="H135" s="24"/>
+      <c r="I135" s="24"/>
+      <c r="J135" s="24"/>
+      <c r="K135" s="24"/>
+      <c r="L135" s="24"/>
+      <c r="M135" s="24"/>
+      <c r="N135" s="24"/>
+      <c r="O135" s="24"/>
+      <c r="P135" s="24"/>
+      <c r="Q135" s="24"/>
+      <c r="R135" s="24"/>
     </row>
     <row r="136" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+      <c r="A136" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B136" s="30"/>
-      <c r="C136" s="30"/>
-      <c r="D136" s="30"/>
-      <c r="E136" s="30"/>
-      <c r="F136" s="30"/>
-      <c r="G136" s="30"/>
-      <c r="H136" s="30"/>
-      <c r="I136" s="30"/>
-      <c r="J136" s="30"/>
-      <c r="K136" s="30"/>
-      <c r="L136" s="30"/>
-      <c r="M136" s="30"/>
-      <c r="N136" s="30"/>
-      <c r="O136" s="30"/>
-      <c r="P136" s="30"/>
-      <c r="Q136" s="30"/>
-      <c r="R136" s="30"/>
-      <c r="S136" s="30"/>
-      <c r="T136" s="30"/>
-      <c r="U136" s="30"/>
-      <c r="V136" s="30"/>
-      <c r="W136" s="30"/>
-      <c r="X136" s="30"/>
-      <c r="Y136" s="30"/>
-      <c r="Z136" s="30"/>
-      <c r="AA136" s="30"/>
+      <c r="B136" s="22"/>
+      <c r="C136" s="22"/>
+      <c r="D136" s="22"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="22"/>
+      <c r="G136" s="22"/>
+      <c r="H136" s="22"/>
+      <c r="I136" s="22"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="22"/>
+      <c r="L136" s="22"/>
+      <c r="M136" s="22"/>
+      <c r="N136" s="22"/>
+      <c r="O136" s="22"/>
+      <c r="P136" s="22"/>
+      <c r="Q136" s="22"/>
+      <c r="R136" s="22"/>
+      <c r="S136" s="22"/>
+      <c r="T136" s="22"/>
+      <c r="U136" s="22"/>
+      <c r="V136" s="22"/>
+      <c r="W136" s="22"/>
+      <c r="X136" s="22"/>
+      <c r="Y136" s="22"/>
+      <c r="Z136" s="22"/>
+      <c r="AA136" s="22"/>
     </row>
     <row r="137" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
@@ -36921,35 +36926,35 @@
       </c>
     </row>
     <row r="153" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A153" s="28" t="s">
+      <c r="A153" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B153" s="28"/>
-      <c r="C153" s="28"/>
-      <c r="D153" s="28"/>
-      <c r="E153" s="28"/>
-      <c r="F153" s="28"/>
-      <c r="G153" s="28"/>
-      <c r="H153" s="28"/>
-      <c r="I153" s="28"/>
-      <c r="J153" s="28"/>
-      <c r="K153" s="28"/>
-      <c r="L153" s="28"/>
-      <c r="M153" s="28"/>
-      <c r="N153" s="28"/>
-      <c r="O153" s="28"/>
-      <c r="P153" s="28"/>
-      <c r="Q153" s="28"/>
-      <c r="R153" s="28"/>
-      <c r="S153" s="28"/>
-      <c r="T153" s="28"/>
-      <c r="U153" s="28"/>
-      <c r="V153" s="28"/>
-      <c r="W153" s="28"/>
-      <c r="X153" s="28"/>
-      <c r="Y153" s="28"/>
-      <c r="Z153" s="28"/>
-      <c r="AA153" s="28"/>
+      <c r="B153" s="23"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="23"/>
+      <c r="E153" s="23"/>
+      <c r="F153" s="23"/>
+      <c r="G153" s="23"/>
+      <c r="H153" s="23"/>
+      <c r="I153" s="23"/>
+      <c r="J153" s="23"/>
+      <c r="K153" s="23"/>
+      <c r="L153" s="23"/>
+      <c r="M153" s="23"/>
+      <c r="N153" s="23"/>
+      <c r="O153" s="23"/>
+      <c r="P153" s="23"/>
+      <c r="Q153" s="23"/>
+      <c r="R153" s="23"/>
+      <c r="S153" s="23"/>
+      <c r="T153" s="23"/>
+      <c r="U153" s="23"/>
+      <c r="V153" s="23"/>
+      <c r="W153" s="23"/>
+      <c r="X153" s="23"/>
+      <c r="Y153" s="23"/>
+      <c r="Z153" s="23"/>
+      <c r="AA153" s="23"/>
     </row>
     <row r="154" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
@@ -38303,55 +38308,55 @@
       </c>
     </row>
     <row r="170" spans="1:35" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="29"/>
-      <c r="B170" s="29"/>
-      <c r="C170" s="29"/>
-      <c r="D170" s="29"/>
-      <c r="E170" s="29"/>
-      <c r="F170" s="29"/>
-      <c r="G170" s="29"/>
-      <c r="H170" s="29"/>
-      <c r="I170" s="29"/>
-      <c r="J170" s="29"/>
-      <c r="K170" s="29"/>
-      <c r="L170" s="29"/>
-      <c r="M170" s="29"/>
-      <c r="N170" s="29"/>
-      <c r="O170" s="29"/>
-      <c r="P170" s="29"/>
-      <c r="Q170" s="29"/>
-      <c r="R170" s="29"/>
+      <c r="A170" s="24"/>
+      <c r="B170" s="24"/>
+      <c r="C170" s="24"/>
+      <c r="D170" s="24"/>
+      <c r="E170" s="24"/>
+      <c r="F170" s="24"/>
+      <c r="G170" s="24"/>
+      <c r="H170" s="24"/>
+      <c r="I170" s="24"/>
+      <c r="J170" s="24"/>
+      <c r="K170" s="24"/>
+      <c r="L170" s="24"/>
+      <c r="M170" s="24"/>
+      <c r="N170" s="24"/>
+      <c r="O170" s="24"/>
+      <c r="P170" s="24"/>
+      <c r="Q170" s="24"/>
+      <c r="R170" s="24"/>
     </row>
     <row r="171" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A171" s="30" t="s">
+      <c r="A171" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B171" s="30"/>
-      <c r="C171" s="30"/>
-      <c r="D171" s="30"/>
-      <c r="E171" s="30"/>
-      <c r="F171" s="30"/>
-      <c r="G171" s="30"/>
-      <c r="H171" s="30"/>
-      <c r="I171" s="30"/>
-      <c r="J171" s="30"/>
-      <c r="K171" s="30"/>
-      <c r="L171" s="30"/>
-      <c r="M171" s="30"/>
-      <c r="N171" s="30"/>
-      <c r="O171" s="30"/>
-      <c r="P171" s="30"/>
-      <c r="Q171" s="30"/>
-      <c r="R171" s="30"/>
-      <c r="S171" s="30"/>
-      <c r="T171" s="30"/>
-      <c r="U171" s="30"/>
-      <c r="V171" s="30"/>
-      <c r="W171" s="30"/>
-      <c r="X171" s="30"/>
-      <c r="Y171" s="30"/>
-      <c r="Z171" s="30"/>
-      <c r="AA171" s="30"/>
+      <c r="B171" s="22"/>
+      <c r="C171" s="22"/>
+      <c r="D171" s="22"/>
+      <c r="E171" s="22"/>
+      <c r="F171" s="22"/>
+      <c r="G171" s="22"/>
+      <c r="H171" s="22"/>
+      <c r="I171" s="22"/>
+      <c r="J171" s="22"/>
+      <c r="K171" s="22"/>
+      <c r="L171" s="22"/>
+      <c r="M171" s="22"/>
+      <c r="N171" s="22"/>
+      <c r="O171" s="22"/>
+      <c r="P171" s="22"/>
+      <c r="Q171" s="22"/>
+      <c r="R171" s="22"/>
+      <c r="S171" s="22"/>
+      <c r="T171" s="22"/>
+      <c r="U171" s="22"/>
+      <c r="V171" s="22"/>
+      <c r="W171" s="22"/>
+      <c r="X171" s="22"/>
+      <c r="Y171" s="22"/>
+      <c r="Z171" s="22"/>
+      <c r="AA171" s="22"/>
     </row>
     <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
@@ -39885,35 +39890,35 @@
       </c>
     </row>
     <row r="190" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A190" s="28" t="s">
+      <c r="A190" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B190" s="28"/>
-      <c r="C190" s="28"/>
-      <c r="D190" s="28"/>
-      <c r="E190" s="28"/>
-      <c r="F190" s="28"/>
-      <c r="G190" s="28"/>
-      <c r="H190" s="28"/>
-      <c r="I190" s="28"/>
-      <c r="J190" s="28"/>
-      <c r="K190" s="28"/>
-      <c r="L190" s="28"/>
-      <c r="M190" s="28"/>
-      <c r="N190" s="28"/>
-      <c r="O190" s="28"/>
-      <c r="P190" s="28"/>
-      <c r="Q190" s="28"/>
-      <c r="R190" s="28"/>
-      <c r="S190" s="28"/>
-      <c r="T190" s="28"/>
-      <c r="U190" s="28"/>
-      <c r="V190" s="28"/>
-      <c r="W190" s="28"/>
-      <c r="X190" s="28"/>
-      <c r="Y190" s="28"/>
-      <c r="Z190" s="28"/>
-      <c r="AA190" s="28"/>
+      <c r="B190" s="23"/>
+      <c r="C190" s="23"/>
+      <c r="D190" s="23"/>
+      <c r="E190" s="23"/>
+      <c r="F190" s="23"/>
+      <c r="G190" s="23"/>
+      <c r="H190" s="23"/>
+      <c r="I190" s="23"/>
+      <c r="J190" s="23"/>
+      <c r="K190" s="23"/>
+      <c r="L190" s="23"/>
+      <c r="M190" s="23"/>
+      <c r="N190" s="23"/>
+      <c r="O190" s="23"/>
+      <c r="P190" s="23"/>
+      <c r="Q190" s="23"/>
+      <c r="R190" s="23"/>
+      <c r="S190" s="23"/>
+      <c r="T190" s="23"/>
+      <c r="U190" s="23"/>
+      <c r="V190" s="23"/>
+      <c r="W190" s="23"/>
+      <c r="X190" s="23"/>
+      <c r="Y190" s="23"/>
+      <c r="Z190" s="23"/>
+      <c r="AA190" s="23"/>
     </row>
     <row r="191" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
@@ -41592,6 +41597,43 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="AK92:AV93"/>
+    <mergeCell ref="AK106:AV107"/>
+    <mergeCell ref="BF63:BJ64"/>
+    <mergeCell ref="AQ78:AU78"/>
+    <mergeCell ref="BD78:BH78"/>
+    <mergeCell ref="AJ49:BQ49"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AR50:AV50"/>
+    <mergeCell ref="AY50:BC50"/>
+    <mergeCell ref="BF50:BJ50"/>
+    <mergeCell ref="BM50:BQ50"/>
+    <mergeCell ref="AK63:AO64"/>
+    <mergeCell ref="AR63:AV64"/>
+    <mergeCell ref="AY63:BC64"/>
+    <mergeCell ref="AQ30:AU30"/>
+    <mergeCell ref="BD30:BH30"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="BM2:BQ2"/>
+    <mergeCell ref="AJ1:BQ1"/>
+    <mergeCell ref="AK15:AO16"/>
+    <mergeCell ref="AR15:AV16"/>
+    <mergeCell ref="AY15:BC16"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="AR2:AV2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BF2:BJ2"/>
+    <mergeCell ref="BF15:BJ16"/>
+    <mergeCell ref="A153:AA153"/>
+    <mergeCell ref="A170:R170"/>
+    <mergeCell ref="A171:AA171"/>
+    <mergeCell ref="A190:AA190"/>
+    <mergeCell ref="A91:AA91"/>
+    <mergeCell ref="A104:R104"/>
+    <mergeCell ref="A105:AA105"/>
+    <mergeCell ref="A120:AA120"/>
+    <mergeCell ref="A135:R135"/>
+    <mergeCell ref="A136:AA136"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="A5:AA5"/>
     <mergeCell ref="A78:AA78"/>
@@ -41607,43 +41649,6 @@
     <mergeCell ref="A55:AA55"/>
     <mergeCell ref="A66:AA66"/>
     <mergeCell ref="A77:R77"/>
-    <mergeCell ref="A153:AA153"/>
-    <mergeCell ref="A170:R170"/>
-    <mergeCell ref="A171:AA171"/>
-    <mergeCell ref="A190:AA190"/>
-    <mergeCell ref="A91:AA91"/>
-    <mergeCell ref="A104:R104"/>
-    <mergeCell ref="A105:AA105"/>
-    <mergeCell ref="A120:AA120"/>
-    <mergeCell ref="A135:R135"/>
-    <mergeCell ref="A136:AA136"/>
-    <mergeCell ref="AQ30:AU30"/>
-    <mergeCell ref="BD30:BH30"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="BM2:BQ2"/>
-    <mergeCell ref="AJ1:BQ1"/>
-    <mergeCell ref="AK15:AO16"/>
-    <mergeCell ref="AR15:AV16"/>
-    <mergeCell ref="AY15:BC16"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="AR2:AV2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BF2:BJ2"/>
-    <mergeCell ref="BF15:BJ16"/>
-    <mergeCell ref="BF63:BJ64"/>
-    <mergeCell ref="AQ78:AU78"/>
-    <mergeCell ref="BD78:BH78"/>
-    <mergeCell ref="AJ49:BQ49"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AR50:AV50"/>
-    <mergeCell ref="AY50:BC50"/>
-    <mergeCell ref="BF50:BJ50"/>
-    <mergeCell ref="BM50:BQ50"/>
-    <mergeCell ref="AK63:AO64"/>
-    <mergeCell ref="AR63:AV64"/>
-    <mergeCell ref="AY63:BC64"/>
-    <mergeCell ref="AK92:AV93"/>
-    <mergeCell ref="AK106:AV107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>